<commit_message>
start to explore social care amounts
</commit_message>
<xml_diff>
--- a/data/support/common_cost_types_between_years.xlsx
+++ b/data/support/common_cost_types_between_years.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="375" windowWidth="17955" windowHeight="11790"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="198">
   <si>
     <t>Year</t>
   </si>
@@ -721,8 +721,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,7 +848,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -857,7 +857,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
@@ -984,7 +983,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1019,7 +1017,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1195,21 +1192,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:H191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:C30"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39" customWidth="1"/>
     <col min="2" max="2" width="50.85546875" customWidth="1"/>
     <col min="3" max="3" width="82.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8">
       <c r="B1" t="s">
         <v>191</v>
       </c>
@@ -1232,11 +1229,11 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:8">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D2">
@@ -1255,9 +1252,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12" t="s">
+    <row r="3" spans="2:8">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D3">
@@ -1276,8 +1273,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="4" spans="2:8">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D4">
@@ -1296,11 +1294,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:8">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D5">
@@ -1319,11 +1317,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+    <row r="6" spans="2:8">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D6">
@@ -1342,11 +1340,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+    <row r="7" spans="2:8">
+      <c r="B7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D7">
@@ -1365,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8">
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1388,11 +1386,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="2:8">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D9">
@@ -1411,11 +1409,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+    <row r="10" spans="2:8">
+      <c r="B10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D10">
@@ -1434,8 +1432,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="11" spans="2:8">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D11">
@@ -1454,11 +1453,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+    <row r="12" spans="2:8">
+      <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D12">
@@ -1477,7 +1476,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8">
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1500,8 +1499,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="14" spans="2:8">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D14">
@@ -1520,11 +1520,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+    <row r="15" spans="2:8">
+      <c r="B15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D15">
@@ -1543,11 +1543,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+    <row r="16" spans="2:8">
+      <c r="B16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D16">
@@ -1566,11 +1566,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
+    <row r="17" spans="2:8">
+      <c r="B17" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D17">
@@ -1589,8 +1589,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+    <row r="18" spans="2:8">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D18">
@@ -1609,8 +1610,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="19" spans="2:8">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D19">
@@ -1629,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8">
       <c r="B20" s="7" t="s">
         <v>19</v>
       </c>
@@ -1652,7 +1654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8">
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
@@ -1675,8 +1677,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="22" spans="2:8">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D22">
@@ -1695,11 +1698,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
+    <row r="23" spans="2:8">
+      <c r="B23" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D23">
@@ -1718,11 +1721,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="13" t="s">
+    <row r="24" spans="2:8">
+      <c r="B24" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D24">
@@ -1741,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8">
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1764,8 +1767,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
+    <row r="26" spans="2:8">
+      <c r="B26" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1787,8 +1790,8 @@
         <v>353</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="16"/>
+    <row r="27" spans="2:8">
+      <c r="B27" s="15"/>
       <c r="C27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1808,11 +1811,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
+    <row r="28" spans="2:8">
+      <c r="B28" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D28">
@@ -1831,11 +1834,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="12" t="s">
+    <row r="29" spans="2:8">
+      <c r="B29" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D29">
@@ -1854,7 +1857,8 @@
         <v>353</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8">
+      <c r="B30" s="8"/>
       <c r="C30" s="8" t="s">
         <v>29</v>
       </c>
@@ -1874,7 +1878,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8">
       <c r="B31" s="7" t="s">
         <v>19</v>
       </c>
@@ -1897,7 +1901,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8">
       <c r="B32" s="2" t="s">
         <v>20</v>
       </c>
@@ -1920,7 +1924,8 @@
         <v>353</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8">
+      <c r="B33" s="8"/>
       <c r="C33" s="8" t="s">
         <v>32</v>
       </c>
@@ -1940,7 +1945,8 @@
         <v>353</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8">
+      <c r="B34" s="8"/>
       <c r="C34" s="8" t="s">
         <v>33</v>
       </c>
@@ -1960,11 +1966,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
+    <row r="35" spans="2:8">
+      <c r="B35" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D35">
@@ -1983,8 +1989,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+    <row r="36" spans="2:8">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D36">
@@ -2003,8 +2010,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="37" spans="2:8">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D37">
@@ -2023,11 +2031,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="10" t="s">
+    <row r="38" spans="2:8">
+      <c r="B38" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D38">
@@ -2046,9 +2054,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="12"/>
-      <c r="C39" s="12" t="s">
+    <row r="39" spans="2:8">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D39">
@@ -2067,8 +2075,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+    <row r="40" spans="2:8">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8" t="s">
         <v>39</v>
       </c>
       <c r="D40">
@@ -2087,11 +2096,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
+    <row r="41" spans="2:8">
+      <c r="B41" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D41">
@@ -2110,7 +2119,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8">
       <c r="B42" s="1" t="s">
         <v>193</v>
       </c>
@@ -2133,7 +2142,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8">
       <c r="B43" s="1" t="s">
         <v>193</v>
       </c>
@@ -2156,11 +2165,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="10" t="s">
+    <row r="44" spans="2:8">
+      <c r="B44" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D44">
@@ -2179,7 +2188,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8">
       <c r="C45" t="s">
         <v>44</v>
       </c>
@@ -2199,11 +2208,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="10" t="s">
+    <row r="46" spans="2:8">
+      <c r="B46" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>45</v>
       </c>
       <c r="D46">
@@ -2222,11 +2231,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="10" t="s">
+    <row r="47" spans="2:8">
+      <c r="B47" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>46</v>
       </c>
       <c r="D47">
@@ -2245,7 +2254,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8">
       <c r="B48" s="1" t="s">
         <v>48</v>
       </c>
@@ -2268,7 +2277,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8">
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
@@ -2291,11 +2300,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="10" t="s">
+    <row r="50" spans="2:8">
+      <c r="B50" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="9" t="s">
         <v>49</v>
       </c>
       <c r="D50">
@@ -2314,7 +2323,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8">
       <c r="B51" s="1" t="s">
         <v>51</v>
       </c>
@@ -2337,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8">
       <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
@@ -2360,7 +2369,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8">
       <c r="B53" s="3" t="s">
         <v>194</v>
       </c>
@@ -2383,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8">
       <c r="B54" s="4" t="s">
         <v>195</v>
       </c>
@@ -2406,7 +2415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8">
       <c r="B55" s="5" t="s">
         <v>196</v>
       </c>
@@ -2429,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8">
       <c r="B56" s="3" t="s">
         <v>194</v>
       </c>
@@ -2452,9 +2461,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="9"/>
-      <c r="C57" s="9" t="s">
+    <row r="57" spans="2:8">
+      <c r="B57" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D57">
@@ -2473,7 +2484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8">
       <c r="B58" s="4" t="s">
         <v>195</v>
       </c>
@@ -2496,7 +2507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8">
       <c r="B59" s="5" t="s">
         <v>196</v>
       </c>
@@ -2519,7 +2530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8">
       <c r="B60" s="3" t="s">
         <v>194</v>
       </c>
@@ -2542,7 +2553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8">
       <c r="B61" s="4" t="s">
         <v>195</v>
       </c>
@@ -2565,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8">
       <c r="B62" s="5" t="s">
         <v>196</v>
       </c>
@@ -2588,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8">
       <c r="B63" s="3" t="s">
         <v>194</v>
       </c>
@@ -2611,7 +2622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8">
       <c r="B64" s="4" t="s">
         <v>195</v>
       </c>
@@ -2634,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8">
       <c r="B65" s="5" t="s">
         <v>196</v>
       </c>
@@ -2657,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8">
       <c r="B66" s="3" t="s">
         <v>194</v>
       </c>
@@ -2680,9 +2691,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="9"/>
-      <c r="C67" s="9" t="s">
+    <row r="67" spans="2:8">
+      <c r="B67" s="8"/>
+      <c r="C67" s="8" t="s">
         <v>66</v>
       </c>
       <c r="D67">
@@ -2701,7 +2712,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8">
       <c r="B68" s="4" t="s">
         <v>195</v>
       </c>
@@ -2724,7 +2735,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8">
       <c r="B69" s="3" t="s">
         <v>194</v>
       </c>
@@ -2747,11 +2758,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="10" t="s">
+    <row r="70" spans="2:8">
+      <c r="B70" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C70" s="9" t="s">
         <v>69</v>
       </c>
       <c r="D70">
@@ -2770,8 +2781,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
+    <row r="71" spans="2:8">
+      <c r="B71" s="9"/>
+      <c r="C71" s="9" t="s">
         <v>70</v>
       </c>
       <c r="D71">
@@ -2790,11 +2802,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="10" t="s">
+    <row r="72" spans="2:8">
+      <c r="B72" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="10" t="s">
+      <c r="C72" s="9" t="s">
         <v>71</v>
       </c>
       <c r="D72">
@@ -2813,11 +2825,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="10" t="s">
+    <row r="73" spans="2:8">
+      <c r="B73" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" s="9" t="s">
         <v>72</v>
       </c>
       <c r="D73">
@@ -2836,11 +2848,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="10" t="s">
+    <row r="74" spans="2:8">
+      <c r="B74" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C74" s="9" t="s">
         <v>73</v>
       </c>
       <c r="D74">
@@ -2859,11 +2871,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="10" t="s">
+    <row r="75" spans="2:8">
+      <c r="B75" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C75" s="9" t="s">
         <v>74</v>
       </c>
       <c r="D75">
@@ -2882,11 +2894,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="10" t="s">
+    <row r="76" spans="2:8">
+      <c r="B76" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C76" s="9" t="s">
         <v>75</v>
       </c>
       <c r="D76">
@@ -2905,8 +2917,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
+    <row r="77" spans="2:8">
+      <c r="B77" s="8"/>
+      <c r="C77" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D77">
@@ -2925,8 +2938,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
+    <row r="78" spans="2:8">
+      <c r="B78" s="8"/>
+      <c r="C78" s="8" t="s">
         <v>77</v>
       </c>
       <c r="D78">
@@ -2945,8 +2959,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
+    <row r="79" spans="2:8">
+      <c r="B79" s="8"/>
+      <c r="C79" s="8" t="s">
         <v>78</v>
       </c>
       <c r="D79">
@@ -2965,8 +2980,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
+    <row r="80" spans="2:8">
+      <c r="B80" s="8"/>
+      <c r="C80" s="8" t="s">
         <v>79</v>
       </c>
       <c r="D80">
@@ -2985,8 +3001,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
+    <row r="81" spans="2:8">
+      <c r="B81" s="8"/>
+      <c r="C81" s="8" t="s">
         <v>80</v>
       </c>
       <c r="D81">
@@ -3005,8 +3022,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
+    <row r="82" spans="2:8">
+      <c r="B82" s="8"/>
+      <c r="C82" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D82">
@@ -3025,11 +3043,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="10" t="s">
+    <row r="83" spans="2:8">
+      <c r="B83" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C83" s="9" t="s">
         <v>82</v>
       </c>
       <c r="D83">
@@ -3048,9 +3066,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="9"/>
-      <c r="C84" s="9" t="s">
+    <row r="84" spans="2:8">
+      <c r="B84" s="8"/>
+      <c r="C84" s="8" t="s">
         <v>83</v>
       </c>
       <c r="D84">
@@ -3069,9 +3087,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="9"/>
-      <c r="C85" s="9" t="s">
+    <row r="85" spans="2:8">
+      <c r="B85" s="8"/>
+      <c r="C85" s="8" t="s">
         <v>84</v>
       </c>
       <c r="D85">
@@ -3090,11 +3108,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="10" t="s">
+    <row r="86" spans="2:8">
+      <c r="B86" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C86" s="10" t="s">
+      <c r="C86" s="9" t="s">
         <v>85</v>
       </c>
       <c r="D86">
@@ -3113,9 +3131,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B87" s="9"/>
-      <c r="C87" s="9" t="s">
+    <row r="87" spans="2:8">
+      <c r="B87" s="8"/>
+      <c r="C87" s="8" t="s">
         <v>86</v>
       </c>
       <c r="D87">
@@ -3134,11 +3152,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="10" t="s">
+    <row r="88" spans="2:8">
+      <c r="B88" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C88" s="10" t="s">
+      <c r="C88" s="9" t="s">
         <v>87</v>
       </c>
       <c r="D88">
@@ -3157,11 +3175,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="10" t="s">
+    <row r="89" spans="2:8">
+      <c r="B89" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C89" s="10" t="s">
+      <c r="C89" s="9" t="s">
         <v>88</v>
       </c>
       <c r="D89">
@@ -3180,11 +3198,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="10" t="s">
+    <row r="90" spans="2:8">
+      <c r="B90" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C90" s="10" t="s">
+      <c r="C90" s="9" t="s">
         <v>89</v>
       </c>
       <c r="D90">
@@ -3203,7 +3221,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8">
       <c r="B91" s="1" t="s">
         <v>91</v>
       </c>
@@ -3226,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8">
       <c r="B92" s="1" t="s">
         <v>91</v>
       </c>
@@ -3249,11 +3267,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="10" t="s">
+    <row r="93" spans="2:8">
+      <c r="B93" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C93" s="10" t="s">
+      <c r="C93" s="9" t="s">
         <v>92</v>
       </c>
       <c r="D93">
@@ -3272,7 +3290,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8">
       <c r="B94" s="6" t="s">
         <v>94</v>
       </c>
@@ -3295,7 +3313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8">
       <c r="B95" s="6" t="s">
         <v>94</v>
       </c>
@@ -3318,11 +3336,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="10" t="s">
+    <row r="96" spans="2:8">
+      <c r="B96" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C96" s="9" t="s">
         <v>95</v>
       </c>
       <c r="D96">
@@ -3341,11 +3359,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="10" t="s">
+    <row r="97" spans="2:8">
+      <c r="B97" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C97" s="9" t="s">
         <v>96</v>
       </c>
       <c r="D97">
@@ -3364,8 +3382,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C98" t="s">
+    <row r="98" spans="2:8">
+      <c r="B98" s="8"/>
+      <c r="C98" s="8" t="s">
         <v>97</v>
       </c>
       <c r="D98">
@@ -3384,8 +3403,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C99" t="s">
+    <row r="99" spans="2:8">
+      <c r="B99" s="9"/>
+      <c r="C99" s="9" t="s">
         <v>98</v>
       </c>
       <c r="D99">
@@ -3404,7 +3424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:8">
       <c r="B100" s="6" t="s">
         <v>100</v>
       </c>
@@ -3427,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:8">
       <c r="B101" s="6" t="s">
         <v>100</v>
       </c>
@@ -3450,11 +3470,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B102" s="10" t="s">
+    <row r="102" spans="2:8">
+      <c r="B102" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C102" s="10" t="s">
+      <c r="C102" s="9" t="s">
         <v>101</v>
       </c>
       <c r="D102">
@@ -3473,9 +3493,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B103" s="9"/>
-      <c r="C103" s="9" t="s">
+    <row r="103" spans="2:8">
+      <c r="B103" s="8"/>
+      <c r="C103" s="8" t="s">
         <v>102</v>
       </c>
       <c r="D103">
@@ -3494,9 +3514,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B104" s="9"/>
-      <c r="C104" s="9" t="s">
+    <row r="104" spans="2:8">
+      <c r="B104" s="8"/>
+      <c r="C104" s="8" t="s">
         <v>103</v>
       </c>
       <c r="D104">
@@ -3515,9 +3535,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B105" s="9"/>
-      <c r="C105" s="9" t="s">
+    <row r="105" spans="2:8">
+      <c r="B105" s="8"/>
+      <c r="C105" s="8" t="s">
         <v>104</v>
       </c>
       <c r="D105">
@@ -3536,9 +3556,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B106" s="9"/>
-      <c r="C106" s="9" t="s">
+    <row r="106" spans="2:8">
+      <c r="B106" s="8"/>
+      <c r="C106" s="8" t="s">
         <v>105</v>
       </c>
       <c r="D106">
@@ -3557,9 +3577,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B107" s="9"/>
-      <c r="C107" s="9" t="s">
+    <row r="107" spans="2:8">
+      <c r="B107" s="8"/>
+      <c r="C107" s="8" t="s">
         <v>106</v>
       </c>
       <c r="D107">
@@ -3578,9 +3598,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B108" s="9"/>
-      <c r="C108" s="9" t="s">
+    <row r="108" spans="2:8">
+      <c r="B108" s="8"/>
+      <c r="C108" s="8" t="s">
         <v>107</v>
       </c>
       <c r="D108">
@@ -3599,9 +3619,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B109" s="9"/>
-      <c r="C109" s="9" t="s">
+    <row r="109" spans="2:8">
+      <c r="B109" s="8"/>
+      <c r="C109" s="8" t="s">
         <v>108</v>
       </c>
       <c r="D109">
@@ -3620,9 +3640,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B110" s="9"/>
-      <c r="C110" s="9" t="s">
+    <row r="110" spans="2:8">
+      <c r="B110" s="8"/>
+      <c r="C110" s="8" t="s">
         <v>109</v>
       </c>
       <c r="D110">
@@ -3641,9 +3661,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B111" s="9"/>
-      <c r="C111" s="9" t="s">
+    <row r="111" spans="2:8">
+      <c r="B111" s="8"/>
+      <c r="C111" s="8" t="s">
         <v>110</v>
       </c>
       <c r="D111">
@@ -3662,9 +3682,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B112" s="9"/>
-      <c r="C112" s="9" t="s">
+    <row r="112" spans="2:8">
+      <c r="B112" s="8"/>
+      <c r="C112" s="8" t="s">
         <v>111</v>
       </c>
       <c r="D112">
@@ -3683,9 +3703,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B113" s="9"/>
-      <c r="C113" s="9" t="s">
+    <row r="113" spans="2:8">
+      <c r="B113" s="8"/>
+      <c r="C113" s="8" t="s">
         <v>112</v>
       </c>
       <c r="D113">
@@ -3704,9 +3724,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B114" s="9"/>
-      <c r="C114" s="9" t="s">
+    <row r="114" spans="2:8">
+      <c r="B114" s="8"/>
+      <c r="C114" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D114">
@@ -3725,9 +3745,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B115" s="9"/>
-      <c r="C115" s="9" t="s">
+    <row r="115" spans="2:8">
+      <c r="B115" s="8"/>
+      <c r="C115" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D115">
@@ -3746,9 +3766,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B116" s="9"/>
-      <c r="C116" s="9" t="s">
+    <row r="116" spans="2:8">
+      <c r="B116" s="8"/>
+      <c r="C116" s="8" t="s">
         <v>115</v>
       </c>
       <c r="D116">
@@ -3767,9 +3787,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B117" s="9"/>
-      <c r="C117" s="9" t="s">
+    <row r="117" spans="2:8">
+      <c r="B117" s="8"/>
+      <c r="C117" s="8" t="s">
         <v>116</v>
       </c>
       <c r="D117">
@@ -3788,9 +3808,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B118" s="9"/>
-      <c r="C118" s="9" t="s">
+    <row r="118" spans="2:8">
+      <c r="B118" s="8"/>
+      <c r="C118" s="8" t="s">
         <v>117</v>
       </c>
       <c r="D118">
@@ -3809,9 +3829,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B119" s="9"/>
-      <c r="C119" s="9" t="s">
+    <row r="119" spans="2:8">
+      <c r="B119" s="8"/>
+      <c r="C119" s="8" t="s">
         <v>118</v>
       </c>
       <c r="D119">
@@ -3830,9 +3850,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B120" s="9"/>
-      <c r="C120" s="9" t="s">
+    <row r="120" spans="2:8">
+      <c r="B120" s="8"/>
+      <c r="C120" s="8" t="s">
         <v>119</v>
       </c>
       <c r="D120">
@@ -3851,9 +3871,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="9"/>
-      <c r="C121" s="9" t="s">
+    <row r="121" spans="2:8">
+      <c r="B121" s="8"/>
+      <c r="C121" s="8" t="s">
         <v>120</v>
       </c>
       <c r="D121">
@@ -3872,9 +3892,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B122" s="9"/>
-      <c r="C122" s="9" t="s">
+    <row r="122" spans="2:8">
+      <c r="B122" s="8"/>
+      <c r="C122" s="8" t="s">
         <v>121</v>
       </c>
       <c r="D122">
@@ -3893,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:8">
       <c r="B123" s="1" t="s">
         <v>122</v>
       </c>
@@ -3916,9 +3936,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B124" s="9"/>
-      <c r="C124" s="9" t="s">
+    <row r="124" spans="2:8">
+      <c r="B124" s="8"/>
+      <c r="C124" s="8" t="s">
         <v>123</v>
       </c>
       <c r="D124">
@@ -3937,9 +3957,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B125" s="9"/>
-      <c r="C125" s="9" t="s">
+    <row r="125" spans="2:8">
+      <c r="B125" s="8"/>
+      <c r="C125" s="8" t="s">
         <v>124</v>
       </c>
       <c r="D125">
@@ -3958,9 +3978,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="9"/>
-      <c r="C126" s="9" t="s">
+    <row r="126" spans="2:8">
+      <c r="B126" s="8"/>
+      <c r="C126" s="8" t="s">
         <v>125</v>
       </c>
       <c r="D126">
@@ -3979,9 +3999,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B127" s="9"/>
-      <c r="C127" s="9" t="s">
+    <row r="127" spans="2:8">
+      <c r="B127" s="8"/>
+      <c r="C127" s="8" t="s">
         <v>126</v>
       </c>
       <c r="D127">
@@ -4000,9 +4020,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B128" s="9"/>
-      <c r="C128" s="9" t="s">
+    <row r="128" spans="2:8">
+      <c r="B128" s="8"/>
+      <c r="C128" s="8" t="s">
         <v>127</v>
       </c>
       <c r="D128">
@@ -4021,9 +4041,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B129" s="9"/>
-      <c r="C129" s="9" t="s">
+    <row r="129" spans="2:8">
+      <c r="B129" s="8"/>
+      <c r="C129" s="8" t="s">
         <v>128</v>
       </c>
       <c r="D129">
@@ -4042,9 +4062,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B130" s="9"/>
-      <c r="C130" s="9" t="s">
+    <row r="130" spans="2:8">
+      <c r="B130" s="8"/>
+      <c r="C130" s="8" t="s">
         <v>129</v>
       </c>
       <c r="D130">
@@ -4063,9 +4083,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B131" s="9"/>
-      <c r="C131" s="9" t="s">
+    <row r="131" spans="2:8">
+      <c r="B131" s="8"/>
+      <c r="C131" s="8" t="s">
         <v>130</v>
       </c>
       <c r="D131">
@@ -4084,9 +4104,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B132" s="9"/>
-      <c r="C132" s="9" t="s">
+    <row r="132" spans="2:8">
+      <c r="B132" s="8"/>
+      <c r="C132" s="8" t="s">
         <v>131</v>
       </c>
       <c r="D132">
@@ -4105,9 +4125,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B133" s="9"/>
-      <c r="C133" s="9" t="s">
+    <row r="133" spans="2:8">
+      <c r="B133" s="8"/>
+      <c r="C133" s="8" t="s">
         <v>132</v>
       </c>
       <c r="D133">
@@ -4126,9 +4146,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B134" s="9"/>
-      <c r="C134" s="9" t="s">
+    <row r="134" spans="2:8">
+      <c r="B134" s="8"/>
+      <c r="C134" s="8" t="s">
         <v>133</v>
       </c>
       <c r="D134">
@@ -4147,9 +4167,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B135" s="9"/>
-      <c r="C135" s="9" t="s">
+    <row r="135" spans="2:8">
+      <c r="B135" s="8"/>
+      <c r="C135" s="8" t="s">
         <v>134</v>
       </c>
       <c r="D135">
@@ -4168,9 +4188,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B136" s="9"/>
-      <c r="C136" s="9" t="s">
+    <row r="136" spans="2:8">
+      <c r="B136" s="8"/>
+      <c r="C136" s="8" t="s">
         <v>135</v>
       </c>
       <c r="D136">
@@ -4189,9 +4209,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B137" s="9"/>
-      <c r="C137" s="9" t="s">
+    <row r="137" spans="2:8">
+      <c r="B137" s="8"/>
+      <c r="C137" s="8" t="s">
         <v>136</v>
       </c>
       <c r="D137">
@@ -4210,9 +4230,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B138" s="9"/>
-      <c r="C138" s="9" t="s">
+    <row r="138" spans="2:8">
+      <c r="B138" s="8"/>
+      <c r="C138" s="8" t="s">
         <v>137</v>
       </c>
       <c r="D138">
@@ -4231,9 +4251,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B139" s="9"/>
-      <c r="C139" s="9" t="s">
+    <row r="139" spans="2:8">
+      <c r="B139" s="8"/>
+      <c r="C139" s="8" t="s">
         <v>138</v>
       </c>
       <c r="D139">
@@ -4252,9 +4272,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B140" s="9"/>
-      <c r="C140" s="9" t="s">
+    <row r="140" spans="2:8">
+      <c r="B140" s="8"/>
+      <c r="C140" s="8" t="s">
         <v>139</v>
       </c>
       <c r="D140">
@@ -4273,9 +4293,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B141" s="9"/>
-      <c r="C141" s="9" t="s">
+    <row r="141" spans="2:8">
+      <c r="B141" s="8"/>
+      <c r="C141" s="8" t="s">
         <v>140</v>
       </c>
       <c r="D141">
@@ -4294,9 +4314,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B142" s="9"/>
-      <c r="C142" s="9" t="s">
+    <row r="142" spans="2:8">
+      <c r="B142" s="8"/>
+      <c r="C142" s="8" t="s">
         <v>141</v>
       </c>
       <c r="D142">
@@ -4315,9 +4335,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B143" s="9"/>
-      <c r="C143" s="9" t="s">
+    <row r="143" spans="2:8">
+      <c r="B143" s="8"/>
+      <c r="C143" s="8" t="s">
         <v>142</v>
       </c>
       <c r="D143">
@@ -4336,7 +4356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:8">
       <c r="B144" s="1" t="s">
         <v>122</v>
       </c>
@@ -4359,7 +4379,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:8">
       <c r="B145" s="1" t="s">
         <v>146</v>
       </c>
@@ -4382,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:8">
       <c r="B146" s="1" t="s">
         <v>146</v>
       </c>
@@ -4405,7 +4425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:8">
       <c r="B147" s="1" t="s">
         <v>146</v>
       </c>
@@ -4428,9 +4448,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B148" s="9"/>
-      <c r="C148" s="9" t="s">
+    <row r="148" spans="2:8">
+      <c r="B148" s="8"/>
+      <c r="C148" s="8" t="s">
         <v>147</v>
       </c>
       <c r="D148">
@@ -4449,9 +4469,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B149" s="9"/>
-      <c r="C149" s="9" t="s">
+    <row r="149" spans="2:8">
+      <c r="B149" s="8"/>
+      <c r="C149" s="8" t="s">
         <v>148</v>
       </c>
       <c r="D149">
@@ -4470,11 +4490,11 @@
         <v>326</v>
       </c>
     </row>
-    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B150" s="10" t="s">
+    <row r="150" spans="2:8">
+      <c r="B150" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C150" s="10" t="s">
+      <c r="C150" s="9" t="s">
         <v>149</v>
       </c>
       <c r="D150">
@@ -4493,11 +4513,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B151" s="10" t="s">
+    <row r="151" spans="2:8">
+      <c r="B151" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C151" s="10" t="s">
+      <c r="C151" s="9" t="s">
         <v>150</v>
       </c>
       <c r="D151">
@@ -4516,11 +4536,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B152" s="10" t="s">
+    <row r="152" spans="2:8">
+      <c r="B152" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="C152" s="10" t="s">
+      <c r="C152" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D152">
@@ -4539,11 +4559,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B153" s="10" t="s">
+    <row r="153" spans="2:8">
+      <c r="B153" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C153" s="10" t="s">
+      <c r="C153" s="9" t="s">
         <v>152</v>
       </c>
       <c r="D153">
@@ -4562,11 +4582,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B154" s="10" t="s">
+    <row r="154" spans="2:8">
+      <c r="B154" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C154" s="10" t="s">
+      <c r="C154" s="9" t="s">
         <v>153</v>
       </c>
       <c r="D154">
@@ -4585,11 +4605,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B155" s="10" t="s">
+    <row r="155" spans="2:8">
+      <c r="B155" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C155" s="10" t="s">
+      <c r="C155" s="9" t="s">
         <v>154</v>
       </c>
       <c r="D155">
@@ -4608,11 +4628,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="156" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B156" s="10" t="s">
+    <row r="156" spans="2:8">
+      <c r="B156" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C156" s="10" t="s">
+      <c r="C156" s="9" t="s">
         <v>155</v>
       </c>
       <c r="D156">
@@ -4631,10 +4651,13 @@
         <v>353</v>
       </c>
     </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C157" t="s">
+    <row r="157" spans="2:8">
+      <c r="B157" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="C157" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="D157">
         <v>0</v>
       </c>
@@ -4651,11 +4674,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B158" s="10" t="s">
+    <row r="158" spans="2:8">
+      <c r="B158" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C158" s="10" t="s">
+      <c r="C158" s="9" t="s">
         <v>157</v>
       </c>
       <c r="D158">
@@ -4674,11 +4697,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B159" s="10" t="s">
+    <row r="159" spans="2:8">
+      <c r="B159" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C159" s="10" t="s">
+      <c r="C159" s="9" t="s">
         <v>158</v>
       </c>
       <c r="D159">
@@ -4697,11 +4720,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B160" s="10" t="s">
+    <row r="160" spans="2:8">
+      <c r="B160" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="C160" s="10" t="s">
+      <c r="C160" s="9" t="s">
         <v>159</v>
       </c>
       <c r="D160">
@@ -4720,9 +4743,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="161" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B161" s="9"/>
-      <c r="C161" s="9" t="s">
+    <row r="161" spans="2:8">
+      <c r="B161" s="8"/>
+      <c r="C161" s="8" t="s">
         <v>160</v>
       </c>
       <c r="D161">
@@ -4741,8 +4764,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="162" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C162" t="s">
+    <row r="162" spans="2:8">
+      <c r="B162" s="8"/>
+      <c r="C162" s="8" t="s">
         <v>161</v>
       </c>
       <c r="D162">
@@ -4761,8 +4785,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C163" t="s">
+    <row r="163" spans="2:8">
+      <c r="B163" s="8"/>
+      <c r="C163" s="8" t="s">
         <v>162</v>
       </c>
       <c r="D163">
@@ -4781,7 +4806,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="164" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:8">
       <c r="B164" s="1" t="s">
         <v>197</v>
       </c>
@@ -4804,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:8">
       <c r="B165" s="1" t="s">
         <v>197</v>
       </c>
@@ -4827,7 +4852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:8">
       <c r="B166" s="1" t="s">
         <v>197</v>
       </c>
@@ -4850,7 +4875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:8">
       <c r="B167" s="1" t="s">
         <v>197</v>
       </c>
@@ -4873,11 +4898,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="168" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B168" s="10" t="s">
+    <row r="168" spans="2:8">
+      <c r="B168" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C168" s="10" t="s">
+      <c r="C168" s="9" t="s">
         <v>167</v>
       </c>
       <c r="D168">
@@ -4896,8 +4921,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="169" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C169" t="s">
+    <row r="169" spans="2:8">
+      <c r="B169" s="8"/>
+      <c r="C169" s="8" t="s">
         <v>168</v>
       </c>
       <c r="D169">
@@ -4916,8 +4942,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C170" t="s">
+    <row r="170" spans="2:8">
+      <c r="B170" s="8"/>
+      <c r="C170" s="8" t="s">
         <v>169</v>
       </c>
       <c r="D170">
@@ -4936,9 +4963,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B171" s="12"/>
-      <c r="C171" s="12" t="s">
+    <row r="171" spans="2:8">
+      <c r="B171" s="11"/>
+      <c r="C171" s="11" t="s">
         <v>170</v>
       </c>
       <c r="D171">
@@ -4957,11 +4984,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B172" s="10" t="s">
+    <row r="172" spans="2:8">
+      <c r="B172" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="C172" s="10" t="s">
+      <c r="C172" s="9" t="s">
         <v>171</v>
       </c>
       <c r="D172">
@@ -4980,11 +5007,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="173" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B173" s="10" t="s">
+    <row r="173" spans="2:8">
+      <c r="B173" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C173" s="10" t="s">
+      <c r="C173" s="9" t="s">
         <v>172</v>
       </c>
       <c r="D173">
@@ -5003,11 +5030,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="174" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B174" s="10" t="s">
+    <row r="174" spans="2:8">
+      <c r="B174" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C174" s="10" t="s">
+      <c r="C174" s="9" t="s">
         <v>173</v>
       </c>
       <c r="D174">
@@ -5026,8 +5053,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="175" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C175" t="s">
+    <row r="175" spans="2:8">
+      <c r="B175" s="8"/>
+      <c r="C175" s="8" t="s">
         <v>174</v>
       </c>
       <c r="D175">
@@ -5046,8 +5074,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C176" t="s">
+    <row r="176" spans="2:8">
+      <c r="B176" s="8"/>
+      <c r="C176" s="8" t="s">
         <v>175</v>
       </c>
       <c r="D176">
@@ -5066,9 +5095,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B177" s="9"/>
-      <c r="C177" s="9" t="s">
+    <row r="177" spans="2:8">
+      <c r="B177" s="8"/>
+      <c r="C177" s="8" t="s">
         <v>176</v>
       </c>
       <c r="D177">
@@ -5087,9 +5116,9 @@
         <v>242</v>
       </c>
     </row>
-    <row r="178" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B178" s="9"/>
-      <c r="C178" s="9" t="s">
+    <row r="178" spans="2:8">
+      <c r="B178" s="8"/>
+      <c r="C178" s="8" t="s">
         <v>177</v>
       </c>
       <c r="D178">
@@ -5108,9 +5137,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="179" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B179" s="9"/>
-      <c r="C179" s="9" t="s">
+    <row r="179" spans="2:8">
+      <c r="B179" s="8"/>
+      <c r="C179" s="8" t="s">
         <v>178</v>
       </c>
       <c r="D179">
@@ -5129,9 +5158,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="180" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B180" s="9"/>
-      <c r="C180" s="9" t="s">
+    <row r="180" spans="2:8">
+      <c r="B180" s="8"/>
+      <c r="C180" s="8" t="s">
         <v>179</v>
       </c>
       <c r="D180">
@@ -5150,9 +5179,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="181" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B181" s="9"/>
-      <c r="C181" s="9" t="s">
+    <row r="181" spans="2:8">
+      <c r="B181" s="8"/>
+      <c r="C181" s="8" t="s">
         <v>180</v>
       </c>
       <c r="D181">
@@ -5171,7 +5200,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="182" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:8">
       <c r="B182" s="1" t="s">
         <v>181</v>
       </c>
@@ -5194,7 +5223,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="183" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:8">
       <c r="B183" s="1" t="s">
         <v>181</v>
       </c>
@@ -5217,8 +5246,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C184" t="s">
+    <row r="184" spans="2:8">
+      <c r="B184" s="8"/>
+      <c r="C184" s="8" t="s">
         <v>183</v>
       </c>
       <c r="D184">
@@ -5237,8 +5267,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C185" t="s">
+    <row r="185" spans="2:8">
+      <c r="B185" s="8"/>
+      <c r="C185" s="8" t="s">
         <v>184</v>
       </c>
       <c r="D185">
@@ -5257,11 +5288,11 @@
         <v>353</v>
       </c>
     </row>
-    <row r="186" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B186" s="10" t="s">
+    <row r="186" spans="2:8">
+      <c r="B186" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="C186" s="10" t="s">
+      <c r="C186" s="9" t="s">
         <v>185</v>
       </c>
       <c r="D186">
@@ -5280,9 +5311,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="187" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B187" s="9"/>
-      <c r="C187" s="9" t="s">
+    <row r="187" spans="2:8">
+      <c r="B187" s="8"/>
+      <c r="C187" s="8" t="s">
         <v>186</v>
       </c>
       <c r="D187">
@@ -5301,9 +5332,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B188" s="9"/>
-      <c r="C188" s="9" t="s">
+    <row r="188" spans="2:8">
+      <c r="B188" s="8"/>
+      <c r="C188" s="8" t="s">
         <v>187</v>
       </c>
       <c r="D188">
@@ -5322,9 +5353,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B189" s="9"/>
-      <c r="C189" s="9" t="s">
+    <row r="189" spans="2:8">
+      <c r="B189" s="8"/>
+      <c r="C189" s="8" t="s">
         <v>188</v>
       </c>
       <c r="D189">
@@ -5343,9 +5374,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B190" s="9"/>
-      <c r="C190" s="9" t="s">
+    <row r="190" spans="2:8">
+      <c r="B190" s="8"/>
+      <c r="C190" s="8" t="s">
         <v>189</v>
       </c>
       <c r="D190">
@@ -5364,9 +5395,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B191" s="9"/>
-      <c r="C191" s="9" t="s">
+    <row r="191" spans="2:8">
+      <c r="B191" s="8"/>
+      <c r="C191" s="8" t="s">
         <v>190</v>
       </c>
       <c r="D191">
@@ -5403,24 +5434,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>